<commit_message>
WIP_Testeando scrappings de varias ciudades y tuneando el robot a partir de bugs resultantes del testing
</commit_message>
<xml_diff>
--- a/viveros_tepicNAY.xlsx
+++ b/viveros_tepicNAY.xlsx
@@ -568,7 +568,7 @@
         <v>https://www.google.com/maps/place/Viveros+de+Nayarit/@21.5197451,-104.9214866,17z/data=!3m1!4b1!4m6!3m5!1s0x8427366428791445:0x41e765252e88eeb5!8m2!3d21.5197451!4d-104.9214866!16s%2Fg%2F11cndbst5h?authuser=0&amp;hl=es</v>
       </c>
       <c r="U2" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.692913632044!2d-104.9214866!3d21.519745099999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427366428791445%3A0x41e765252e88eeb5!2sViveros%20de%20Nayarit!5e0!3m2!1ses!2smx!4v1681320160310!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.692913632044!2d-104.9214866!3d21.519745099999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427366428791445%3A0x41e765252e88eeb5!2sViveros%20de%20Nayarit!5e0!3m2!1ses!2smx!4v1681340140956!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V2" t="str">
         <v>G39H+VC Tepic, Nayarit</v>
@@ -630,10 +630,10 @@
         <v>Av. Tecnológico 2620, Valle de Matatipac, 63195 Tepic, Nay.</v>
       </c>
       <c r="F3" t="str">
-        <v>F4GM+FM Tepic, Nayarit</v>
+        <v>311 213 6510</v>
       </c>
       <c r="G3" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="I3" t="str">
         <v>Miércoles de 08:00 a 19:30,Jueves de 08:00 a 19:30,Viernes de 08:00 a 19:30,Sábado de 08:00 a 19:30,Domingo de 08:00 a 19:30,Lunes de 08:00 a 19:30,Martes de 08:00 a 19:30</v>
@@ -660,7 +660,7 @@
         <v>Domingo de 08:00 a 19:30</v>
       </c>
       <c r="Q3" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R3" t="str">
         <v>tepic</v>
@@ -672,10 +672,10 @@
         <v>https://www.google.com/maps/place/Vivero+Paraiso/@21.4761576,-104.8658628,17z/data=!3m1!4b1!4m6!3m5!1s0x842737497e06b2c7:0x93ff353e43b4c9d5!8m2!3d21.4761576!4d-104.8658628!16s%2Fg%2F11cnctsrx5?authuser=0&amp;hl=es</v>
       </c>
       <c r="U3" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.8052303043883!2d-104.8658628!3d21.4761576!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842737497e06b2c7%3A0x93ff353e43b4c9d5!2sVivero%20Paraiso!5e0!3m2!1ses!2smx!4v1681320166333!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.8052303043883!2d-104.8658628!3d21.4761576!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842737497e06b2c7%3A0x93ff353e43b4c9d5!2sVivero%20Paraiso!5e0!3m2!1ses!2smx!4v1681340146770!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V3" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>F4GM+FM Tepic, Nayarit</v>
       </c>
       <c r="W3" t="str">
         <v>4.3</v>
@@ -734,10 +734,10 @@
         <v>Av. Tecnológico 2590, Valle de Matatipac, 63195 Tepic, Nay.</v>
       </c>
       <c r="F4" t="str">
-        <v>F4GJ+QV Tepic, Nayarit</v>
+        <v>311 129 0239</v>
       </c>
       <c r="G4" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="I4" t="str">
         <v>Miércoles de 08:00 a 18:00,Jueves de 08:00 a 18:00,Viernes de 08:00 a 18:00,Sábado de 08:00 a 18:00,Domingo de 10:00 a 14:00,Lunes de 08:00 a 18:00,Martes de 08:00 a 18:00</v>
@@ -764,7 +764,7 @@
         <v>Domingo de 10:00 a 14:00</v>
       </c>
       <c r="Q4" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R4" t="str">
         <v>tepic</v>
@@ -776,10 +776,10 @@
         <v>https://www.google.com/maps/place/Vivero+Paola/@21.4769553,-104.8678547,17z/data=!3m1!4b1!4m6!3m5!1s0x84273749ee8cae83:0x134a4bce5437328a!8m2!3d21.4769553!4d-104.8678547!16s%2Fg%2F11c0pjk7bv?authuser=0&amp;hl=es</v>
       </c>
       <c r="U4" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.7848929654606!2d-104.8678547!3d21.4769553!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273749ee8cae83%3A0x134a4bce5437328a!2sVivero%20Paola!5e0!3m2!1ses!2smx!4v1681320171510!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.7848929654606!2d-104.8678547!3d21.4769553!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273749ee8cae83%3A0x134a4bce5437328a!2sVivero%20Paola!5e0!3m2!1ses!2smx!4v1681340151486!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V4" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>F4GJ+QV Tepic, Nayarit</v>
       </c>
       <c r="W4" t="str">
         <v>4.9</v>
@@ -880,7 +880,7 @@
         <v>https://www.google.com/maps/place/Vivero+del+Centro+el+Sauce/@21.5113792,-104.8944944,17z/data=!3m1!4b1!4m6!3m5!1s0x8427374b5cccc13b:0x48124671e3225142!8m2!3d21.5113792!4d-104.8944944!16s%2Fg%2F11nm9q9_j5?authuser=0&amp;hl=es</v>
       </c>
       <c r="U5" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.9065710257332!2d-104.8944944!3d21.5113792!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427374b5cccc13b%3A0x48124671e3225142!2sVivero%20del%20Centro%20el%20Sauce!5e0!3m2!1ses!2smx!4v1681320175445!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.9065710257332!2d-104.8944944!3d21.5113792!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427374b5cccc13b%3A0x48124671e3225142!2sVivero%20del%20Centro%20el%20Sauce!5e0!3m2!1ses!2smx!4v1681340156310!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V5" t="str">
         <v>G464+H6 Tepic, Nayarit</v>
@@ -942,10 +942,10 @@
         <v>Av. México Nte. 569, Mololoa, 63050 Tepic, Nay.</v>
       </c>
       <c r="F6" t="str">
-        <v>G496+88 Tepic, Nayarit</v>
+        <v>311 199 3811</v>
       </c>
       <c r="G6" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="I6" t="str">
         <v>Miércoles de 10:00 a 18:00,Jueves de 10:00 a 18:00,Viernes de 10:00 a 18:00,Sábado de 10:00 a 14:00,Domingo Cerrado,Lunes de 10:00 a 18:00,Martes de 10:00 a 18:00</v>
@@ -972,7 +972,7 @@
         <v>Domingo Cerrado</v>
       </c>
       <c r="Q6" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R6" t="str">
         <v>tepic</v>
@@ -984,10 +984,10 @@
         <v>https://www.google.com/maps/place/Vivero+OASIS/@21.5183311,-104.8892192,17z/data=!3m1!4b1!4m6!3m5!1s0x842737aba81b4873:0x359073ef3549ac82!8m2!3d21.5183311!4d-104.8892192!16s%2Fg%2F11df242_k6?authuser=0&amp;hl=es</v>
       </c>
       <c r="U6" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.7290314491374!2d-104.8892192!3d21.518331099999997!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842737aba81b4873%3A0x359073ef3549ac82!2sVivero%20OASIS!5e0!3m2!1ses!2smx!4v1681320179724!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.7290314491374!2d-104.8892192!3d21.518331099999997!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842737aba81b4873%3A0x359073ef3549ac82!2sVivero%20OASIS!5e0!3m2!1ses!2smx!4v1681340160270!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V6" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>G496+88 Tepic, Nayarit</v>
       </c>
       <c r="W6" t="str">
         <v>4.5</v>
@@ -1046,10 +1046,10 @@
         <v>Blvd. Tepic-Xalisco 492, Miravalles, 63184 Tepic, Nay.</v>
       </c>
       <c r="F7" t="str">
-        <v>F4M4+6Q Tepic, Nayarit</v>
+        <v>311 214 0588</v>
       </c>
       <c r="G7" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="I7" t="str">
         <v>Miércoles de 08:00 a 18:00,Jueves de 08:00 a 18:00,Viernes de 08:00 a 18:00,Sábado de 08:00 a 15:00,Domingo Cerrado,Lunes de 08:00 a 18:00,Martes de 08:00 a 18:00</v>
@@ -1076,7 +1076,7 @@
         <v>Domingo Cerrado</v>
       </c>
       <c r="Q7" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R7" t="str">
         <v>tepic</v>
@@ -1088,10 +1088,10 @@
         <v>https://www.google.com/maps/place/El+Bamb%C3%BA/@21.4830549,-104.8930722,17z/data=!3m1!4b1!4m6!3m5!1s0x84273723e33b27e7:0x4a8b9c284bab67c2!8m2!3d21.4830549!4d-104.8930722!16s%2Fg%2F1tkmmwkz?authuser=0&amp;hl=es</v>
       </c>
       <c r="U7" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.62936004577!2d-104.89307219999999!3d21.483054899999996!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273723e33b27e7%3A0x4a8b9c284bab67c2!2zRWwgQmFtYsO6!5e0!3m2!1ses!2smx!4v1681320184570!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.62936004577!2d-104.89307219999999!3d21.483054899999996!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273723e33b27e7%3A0x4a8b9c284bab67c2!2zRWwgQmFtYsO6!5e0!3m2!1ses!2smx!4v1681340165069!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V7" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>F4M4+6Q Tepic, Nayarit</v>
       </c>
       <c r="W7" t="str">
         <v>4.3</v>
@@ -1192,7 +1192,7 @@
         <v>https://www.google.com/maps/place/Vivero+Aguamilpa+%22La+G%C3%BCerita%22/@21.4829002,-104.8448768,17z/data=!3m1!4b1!4m6!3m5!1s0x8427393db26fa1d3:0xac24f604c867f2a0!8m2!3d21.4829002!4d-104.8448768!16s%2Fg%2F11fr935w4q?authuser=0&amp;hl=es</v>
       </c>
       <c r="U8" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.6333052413224!2d-104.8448768!3d21.4829002!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427393db26fa1d3%3A0xac24f604c867f2a0!2sVivero%20Aguamilpa%20%22La%20G%C3%BCerita%22!5e0!3m2!1ses!2smx!4v1681320188714!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.6333052413224!2d-104.8448768!3d21.4829002!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427393db26fa1d3%3A0xac24f604c867f2a0!2sVivero%20Aguamilpa%20%22La%20G%C3%BCerita%22!5e0!3m2!1ses!2smx!4v1681340169902!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V8" t="str">
         <v>F5M4+52 Tepic, Nayarit</v>
@@ -1254,10 +1254,10 @@
         <v>Cactus y suculentas, Ideales de La Justicia 83, 2 de Agosto, 63175 Tepic, Nay.</v>
       </c>
       <c r="F9" t="str">
-        <v>F4JM+J5 Tepic, Nayarit</v>
+        <v>311 202 1219</v>
       </c>
       <c r="G9" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="I9" t="str">
         <v>Miércoles de 09:00 a 19:00,Jueves de 09:00 a 19:00,Viernes de 09:00 a 19:00,Sábado de 09:00 a 19:00,Domingo de 09:00 a 17:00,Lunes de 09:00 a 19:00,Martes de 09:00 a 19:00</v>
@@ -1284,7 +1284,7 @@
         <v>Domingo de 09:00 a 17:00</v>
       </c>
       <c r="Q9" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R9" t="str">
         <v>tepic</v>
@@ -1296,10 +1296,10 @@
         <v>https://www.google.com/maps/place/Cactus+y+suculentas+tepic/@21.4815307,-104.8670522,17z/data=!3m1!4b1!4m6!3m5!1s0x842731bf60888eb3:0xfc13e9e9d5800fe3!8m2!3d21.4815307!4d-104.8670522!16s%2Fg%2F11ft_09hk5?authuser=0&amp;hl=es</v>
       </c>
       <c r="U9" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.6682293700105!2d-104.86705219999999!3d21.4815307!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842731bf60888eb3%3A0xfc13e9e9d5800fe3!2sCactus%20y%20suculentas%20tepic!5e0!3m2!1ses!2smx!4v1681320193114!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.6682293700105!2d-104.86705219999999!3d21.4815307!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842731bf60888eb3%3A0xfc13e9e9d5800fe3!2sCactus%20y%20suculentas%20tepic!5e0!3m2!1ses!2smx!4v1681340174518!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V9" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>F4JM+J5 Tepic, Nayarit</v>
       </c>
       <c r="W9" t="str">
         <v>4.8</v>
@@ -1311,13 +1311,13 @@
         <v>Quedé encantada y sorprendida con tanta variedad de suculentas,Excelente servicio,Gran gran variedad de plantas: arbustos, cactus, suculentas, flores y demás... Muy buena atención de todos los trabajadores y los precios están por abajo comparado con otros viveros. Recomendado</v>
       </c>
       <c r="Z9" t="str">
-        <v>https://lh5.googleusercontent.com/p/AF1QipPnftxscke4s5e9_6nXW347gKV2KlA2s703DZfn=w408-h906-k-no</v>
+        <v>https://lh5.googleusercontent.com/p/AF1QipOoDCqWVVXw4yAySiWx8rA53b5u0FUNUeql72Xl=w408-h905-k-no</v>
       </c>
       <c r="AA9" t="str">
-        <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipPnftxscke4s5e9_6nXW347gKV2KlA2s703DZfn=w408-h906-k-no</v>
+        <v>wget --no-check-certificate https://lh5.googleusercontent.com/p/AF1QipOoDCqWVVXw4yAySiWx8rA53b5u0FUNUeql72Xl=w408-h905-k-no</v>
       </c>
       <c r="AB9" t="str">
-        <v>AF1QipPnftxscke4s5e9_6nXW347gKV2KlA2s703DZfn=w408-h906-k-no</v>
+        <v>AF1QipOoDCqWVVXw4yAySiWx8rA53b5u0FUNUeql72Xl=w408-h905-k-no</v>
       </c>
       <c r="AC9" t="str">
         <v>Cactus_y_suculentas_tepic_7</v>
@@ -1332,7 +1332,7 @@
         <v>https://tierradeplantas.com/wp-content/uploads/2023/04/Cactus_y_suculentas_tepic_7.jpg</v>
       </c>
       <c r="AG9" t="str">
-        <v>ren "AF1QipPnftxscke4s5e9_6nXW347gKV2KlA2s703DZfn=w408-h906-k-no" "Cactus_y_suculentas_tepic_7.jpg"</v>
+        <v>ren "AF1QipOoDCqWVVXw4yAySiWx8rA53b5u0FUNUeql72Xl=w408-h905-k-no" "Cactus_y_suculentas_tepic_7.jpg"</v>
       </c>
       <c r="AH9" t="str">
         <v>viveros-en-tepic-nayarit</v>
@@ -1400,7 +1400,7 @@
         <v>https://www.google.com/maps/place/Vivero+las+margaritas/@21.4701356,-104.8825045,17z/data=!3m1!4b1!4m6!3m5!1s0x8427372d3d1aafcf:0x694bcdf58ee7f191!8m2!3d21.4701356!4d-104.8825045!16s%2Fg%2F11bzt1m8v6?authuser=0&amp;hl=es</v>
       </c>
       <c r="U10" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.958737799926!2d-104.8825045!3d21.4701356!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427372d3d1aafcf%3A0x694bcdf58ee7f191!2sVivero%20las%20margaritas!5e0!3m2!1ses!2smx!4v1681320197662!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.958737799926!2d-104.8825045!3d21.4701356!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427372d3d1aafcf%3A0x694bcdf58ee7f191!2sVivero%20las%20margaritas!5e0!3m2!1ses!2smx!4v1681340178335!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V10" t="str">
         <v>F4C8+3X Tepic, Nayarit</v>
@@ -1462,10 +1462,10 @@
         <v>Roble 33, Los Sauces (Reserva Territorial), Los Sauces, 63197 Tepic, Nay.</v>
       </c>
       <c r="F11" t="str">
-        <v>F49G+3F Tepic, Nayarit</v>
+        <v>311 129 1390</v>
       </c>
       <c r="G11" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="I11" t="str">
         <v>Miércoles de 09:00 a 18:00,Jueves de 09:00 a 18:00,Viernes de 09:00 a 18:00,Sábado de 08:30 a 17:30,Domingo Cerrado,Lunes de 09:00 a 18:00,Martes de 09:00 a 18:00</v>
@@ -1492,7 +1492,7 @@
         <v>Domingo Cerrado</v>
       </c>
       <c r="Q11" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R11" t="str">
         <v>tepic</v>
@@ -1504,10 +1504,10 @@
         <v>https://www.google.com/maps/place/Vivero+Paraiso/@21.4676275,-104.8738573,17z/data=!3m1!4b1!4m6!3m5!1s0x842730cb6f773953:0xca573bda8de1202e!8m2!3d21.4676275!4d-104.8738573!16s%2Fg%2F11cncwy33y?authuser=0&amp;hl=es</v>
       </c>
       <c r="U11" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3713.0226599671323!2d-104.8738573!3d21.4676275!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842730cb6f773953%3A0xca573bda8de1202e!2sVivero%20Paraiso!5e0!3m2!1ses!2smx!4v1681320202760!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3713.0226599671323!2d-104.8738573!3d21.4676275!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842730cb6f773953%3A0xca573bda8de1202e!2sVivero%20Paraiso!5e0!3m2!1ses!2smx!4v1681340182755!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V11" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>F49G+3F Tepic, Nayarit</v>
       </c>
       <c r="W11" t="str">
         <v>0.0</v>
@@ -1566,10 +1566,10 @@
         <v>Fresno 126, San Juan, 63130 Tepic, Nay.</v>
       </c>
       <c r="F12" t="str">
-        <v>G36R+7H Tepic, Nayarit</v>
+        <v>311 122 0902</v>
       </c>
       <c r="G12" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="H12" t="str">
         <v>No se cuenta con horario oficial</v>
@@ -1578,7 +1578,7 @@
         <v>No se cuenta con horario oficial</v>
       </c>
       <c r="Q12" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R12" t="str">
         <v>tepic</v>
@@ -1590,10 +1590,10 @@
         <v>https://www.google.com/maps/place/Viveros+Villanueva/@21.5106924,-104.9085307,17z/data=!3m1!4b1!4m6!3m5!1s0x842736f6666e8c39:0xa427685616ad2b4a!8m2!3d21.5106924!4d-104.9085307!16s%2Fg%2F11b_3h0q28?authuser=0&amp;hl=es</v>
       </c>
       <c r="U12" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.924107751254!2d-104.9085307!3d21.5106924!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842736f6666e8c39%3A0xa427685616ad2b4a!2sViveros%20Villanueva!5e0!3m2!1ses!2smx!4v1681320206964!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.924107751254!2d-104.9085307!3d21.5106924!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842736f6666e8c39%3A0xa427685616ad2b4a!2sViveros%20Villanueva!5e0!3m2!1ses!2smx!4v1681340187938!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V12" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>G36R+7H Tepic, Nayarit</v>
       </c>
       <c r="W12" t="str">
         <v>0.0</v>
@@ -1694,7 +1694,7 @@
         <v>https://www.google.com/maps/place/Vivero+Los+Helechos/@21.4928115,-104.830516,17z/data=!3m1!4b1!4m6!3m5!1s0x84273989522ec1f9:0x40a05e871e85db7!8m2!3d21.4928115!4d-104.830516!16s%2Fg%2F11rj42shwr?authuser=0&amp;hl=es</v>
       </c>
       <c r="U13" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.3804902728566!2d-104.83051599999999!3d21.492811499999995!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273989522ec1f9%3A0x40a05e871e85db7!2sVivero%20Los%20Helechos!5e0!3m2!1ses!2smx!4v1681320211636!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.3804902728566!2d-104.83051599999999!3d21.492811499999995!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273989522ec1f9%3A0x40a05e871e85db7!2sVivero%20Los%20Helechos!5e0!3m2!1ses!2smx!4v1681340192343!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V13" t="str">
         <v>F5V9+4Q Tepic, Nayarit</v>
@@ -1798,7 +1798,7 @@
         <v>https://www.google.com/maps/place/Vivero/@21.5075836,-104.8954181,17z/data=!3m1!4b1!4m6!3m5!1s0x8427379212b7b909:0x665aea3b687c9a85!8m2!3d21.5075836!4d-104.8954181!16s%2Fg%2F11rjvkz19z?authuser=0&amp;hl=es</v>
       </c>
       <c r="U14" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.003481063087!2d-104.8954181!3d21.5075836!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427379212b7b909%3A0x665aea3b687c9a85!2sVivero!5e0!3m2!1ses!2smx!4v1681320215855!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.003481063087!2d-104.8954181!3d21.5075836!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427379212b7b909%3A0x665aea3b687c9a85!2sVivero!5e0!3m2!1ses!2smx!4v1681340196138!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V14" t="str">
         <v>G453+2R Tepic, Nayarit</v>
@@ -1902,7 +1902,7 @@
         <v>https://www.google.com/maps/place/Viveros+villanueva/@21.5054695,-104.9106822,17z/data=!3m1!4b1!4m6!3m5!1s0x8427377c1cf787cd:0x4baa9eec8072ae46!8m2!3d21.5054695!4d-104.9106822!16s%2Fg%2F11jbk377nq?authuser=0&amp;hl=es</v>
       </c>
       <c r="U15" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.0574516341685!2d-104.9106822!3d21.505469500000004!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427377c1cf787cd%3A0x4baa9eec8072ae46!2sViveros%20villanueva!5e0!3m2!1ses!2smx!4v1681320220149!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.0574516341685!2d-104.9106822!3d21.505469500000004!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427377c1cf787cd%3A0x4baa9eec8072ae46!2sViveros%20villanueva!5e0!3m2!1ses!2smx!4v1681340201806!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V15" t="str">
         <v>G34Q+5P Tepic, Nayarit</v>
@@ -2007,7 +2007,7 @@
         <v>https://www.google.com/maps/place/VIVERO+EL+SAUCE/@21.4546802,-104.8218842,17z/data=!3m1!4b1!4m6!3m5!1s0x84265a48266b2605:0xf6a9bb7cee3f7e65!8m2!3d21.4546802!4d-104.8218842!16s%2Fg%2F11tf1plqg3?authuser=0&amp;hl=es</v>
       </c>
       <c r="U16" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3713.352525458845!2d-104.8218842!3d21.4546802!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84265a48266b2605%3A0xf6a9bb7cee3f7e65!2sVIVERO%20EL%20SAUCE!5e0!3m2!1ses!2smx!4v1681320224602!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3713.352525458845!2d-104.8218842!3d21.4546802!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84265a48266b2605%3A0xf6a9bb7cee3f7e65!2sVIVERO%20EL%20SAUCE!5e0!3m2!1ses!2smx!4v1681340207550!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V16" t="str">
         <v>F53H+V6 San Cayetano, Nayarit</v>
@@ -2111,7 +2111,7 @@
         <v>https://www.google.com/maps/place/Vivero+El+Hidalguense/@21.5141706,-104.9044491,17z/data=!3m1!4b1!4m6!3m5!1s0x842736581ac2f859:0x749efba76ad59b03!8m2!3d21.5141706!4d-104.9044491!16s%2Fg%2F11bzthg8pm?authuser=0&amp;hl=es</v>
       </c>
       <c r="U17" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.835290033463!2d-104.9044491!3d21.5141706!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842736581ac2f859%3A0x749efba76ad59b03!2sVivero%20El%20Hidalguense!5e0!3m2!1ses!2smx!4v1681320229111!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.835290033463!2d-104.9044491!3d21.5141706!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842736581ac2f859%3A0x749efba76ad59b03!2sVivero%20El%20Hidalguense!5e0!3m2!1ses!2smx!4v1681340213829!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V17" t="str">
         <v>G37W+M6 Tepic, Nayarit</v>
@@ -2215,7 +2215,7 @@
         <v>https://www.google.com/maps/place/Vivero+La+Loma/@21.5063873,-104.8969392,17z/data=!3m1!4b1!4m6!3m5!1s0x842736fc6eaeb575:0x61c9ca47dfbd9492!8m2!3d21.5063873!4d-104.8969392!16s%2Fg%2F11bzz1yv54?authuser=0&amp;hl=es</v>
       </c>
       <c r="U18" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.0340218636816!2d-104.89693919999999!3d21.5063873!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842736fc6eaeb575%3A0x61c9ca47dfbd9492!2sVivero%20La%20Loma!5e0!3m2!1ses!2smx!4v1681320234342!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.0340218636816!2d-104.89693919999999!3d21.5063873!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842736fc6eaeb575%3A0x61c9ca47dfbd9492!2sVivero%20La%20Loma!5e0!3m2!1ses!2smx!4v1681340219015!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V18" t="str">
         <v>G443+H6 Centro, Tepic, Nay.</v>
@@ -2277,10 +2277,10 @@
         <v>63156, Lib. Nogales 10, Colinas del Rey, 63156 Tepic, Nay.</v>
       </c>
       <c r="F19" t="str">
-        <v>F3RW+59 Tepic, Nayarit</v>
+        <v>311 210 2219</v>
       </c>
       <c r="G19" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="I19" t="str">
         <v>Miércoles de 09:00 a 14:00 de 16:00 a 18:00,Jueves de 09:00 a 14:00 de 16:00 a 18:00,Viernes de 09:00 a 14:00 de 16:00 a 18:00,Sábado de 09:00 a 15:00,Domingo Cerrado,Lunes de 09:00 a 14:00 de 16:00 a 18:00,Martes de 09:00 a 14:00 de 16:00 a 18:00</v>
@@ -2307,7 +2307,7 @@
         <v>Domingo Cerrado</v>
       </c>
       <c r="Q19" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R19" t="str">
         <v>tepic</v>
@@ -2319,10 +2319,10 @@
         <v>https://www.google.com/maps/place/Vivero+Las+Palmas/@21.4904677,-104.9040353,17z/data=!3m1!4b1!4m6!3m5!1s0x8427373b3297fabb:0x889bab5b48b2e94!8m2!3d21.4904677!4d-104.9040353!16s%2Fg%2F1tg50r9q?authuser=0&amp;hl=es</v>
       </c>
       <c r="U19" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.4402853678093!2d-104.90403529999999!3d21.490467700000004!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427373b3297fabb%3A0x889bab5b48b2e94!2sVivero%20Las%20Palmas!5e0!3m2!1ses!2smx!4v1681320238423!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.4402853678093!2d-104.90403529999999!3d21.490467700000004!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427373b3297fabb%3A0x889bab5b48b2e94!2sVivero%20Las%20Palmas!5e0!3m2!1ses!2smx!4v1681340222873!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V19" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>F3RW+59 Tepic, Nayarit</v>
       </c>
       <c r="W19" t="str">
         <v>4.3</v>
@@ -2381,10 +2381,10 @@
         <v>P.º de Geranio, Villas del Roble, 63173 Tepic, Nay.</v>
       </c>
       <c r="F20" t="str">
-        <v>F5WG+4R Tepic, Nayarit</v>
+        <v>311 168 0125</v>
       </c>
       <c r="G20" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="I20" t="str">
         <v>Miércoles de 08:00 a 18:00,Jueves de 08:00 a 18:00,Viernes de 08:00 a 18:00,Sábado de 08:00 a 13:00,Domingo de 09:00 a 14:00,Lunes de 08:00 a 18:00,Martes de 08:00 a 18:00</v>
@@ -2411,7 +2411,7 @@
         <v>Domingo de 09:00 a 14:00</v>
       </c>
       <c r="Q20" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R20" t="str">
         <v>tepic</v>
@@ -2423,10 +2423,10 @@
         <v>https://www.google.com/maps/place/Vivero+Armon%C3%ADa/@21.495311,-104.8229259,17z/data=!3m1!4b1!4m6!3m5!1s0x842739253140278b:0xfd90bc8eea43975!8m2!3d21.495311!4d-104.8229259!16s%2Fg%2F11n71f_zn9?authuser=0&amp;hl=es</v>
       </c>
       <c r="U20" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.316716109926!2d-104.8229259!3d21.495310999999994!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842739253140278b%3A0xfd90bc8eea43975!2sVivero%20Armon%C3%ADa!5e0!3m2!1ses!2smx!4v1681320243248!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.316716109926!2d-104.8229259!3d21.495310999999994!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842739253140278b%3A0xfd90bc8eea43975!2sVivero%20Armon%C3%ADa!5e0!3m2!1ses!2smx!4v1681340227701!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V20" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>F5WG+4R Tepic, Nayarit</v>
       </c>
       <c r="W20" t="str">
         <v>5.0</v>
@@ -2528,7 +2528,7 @@
         <v>https://www.google.com/maps/place/Vivero+Guadalupano/@21.4753433,-104.8633214,17z/data=!3m1!4b1!4m6!3m5!1s0x8427374744c1de03:0x88611883bf1a9d3d!8m2!3d21.4753433!4d-104.8633214!16s%2Fg%2F11qsx3mwlm?authuser=0&amp;hl=es</v>
       </c>
       <c r="U21" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.8259901175516!2d-104.8633214!3d21.475343300000002!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427374744c1de03%3A0x88611883bf1a9d3d!2sVivero%20Guadalupano!5e0!3m2!1ses!2smx!4v1681320247479!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.8259901175516!2d-104.8633214!3d21.475343300000002!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427374744c1de03%3A0x88611883bf1a9d3d!2sVivero%20Guadalupano!5e0!3m2!1ses!2smx!4v1681340231453!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V21" t="str">
         <v>F4GP+4M Tepic, Nayarit</v>
@@ -2632,7 +2632,7 @@
         <v>https://www.google.com/maps/place/Viviero+Echeveria/@21.4850819,-104.8801529,17z/data=!3m1!4b1!4m6!3m5!1s0x8427371ea5ee4493:0xe0ea1d96e8ba3556!8m2!3d21.4850819!4d-104.8801529!16s%2Fg%2F11jnpzgmsx?authuser=0&amp;hl=es</v>
       </c>
       <c r="U22" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.577664517424!2d-104.8801529!3d21.485081899999997!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427371ea5ee4493%3A0xe0ea1d96e8ba3556!2sViviero%20Echeveria!5e0!3m2!1ses!2smx!4v1681320252187!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.577664517424!2d-104.8801529!3d21.485081899999997!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427371ea5ee4493%3A0xe0ea1d96e8ba3556!2sViviero%20Echeveria!5e0!3m2!1ses!2smx!4v1681340236426!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V22" t="str">
         <v>F4P9+2W Tepic, Nayarit</v>
@@ -2736,7 +2736,7 @@
         <v>https://www.google.com/maps/place/Vivero+Cristo+Rey/@21.5233274,-104.918539,17z/data=!3m1!4b1!4m6!3m5!1s0x8427371e3ffbb1d1:0x12ce549dceae2790!8m2!3d21.5233274!4d-104.918539!16s%2Fg%2F11gyd8rt0j?authuser=0&amp;hl=es</v>
       </c>
       <c r="U23" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.6014007866634!2d-104.918539!3d21.5233274!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427371e3ffbb1d1%3A0x12ce549dceae2790!2sVivero%20Cristo%20Rey!5e0!3m2!1ses!2smx!4v1681320256676!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.6014007866634!2d-104.918539!3d21.5233274!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427371e3ffbb1d1%3A0x12ce549dceae2790!2sVivero%20Cristo%20Rey!5e0!3m2!1ses!2smx!4v1681340241240!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V23" t="str">
         <v>G3FJ+8H Tepic, Nayarit</v>
@@ -2798,10 +2798,10 @@
         <v>Hipocampo 5, Rodeo de la Punta, 63110 Tepic, Nay.</v>
       </c>
       <c r="F24" t="str">
-        <v>G38J+54 Tepic, Nayarit</v>
+        <v>311 139 8960</v>
       </c>
       <c r="G24" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="I24" t="str">
         <v>Miércoles de 09:00 a 19:00,Jueves de 09:00 a 19:00,Viernes de 09:00 a 19:00,Sábado de 09:00 a 19:00,Domingo Cerrado,Lunes de 09:00 a 19:00,Martes de 09:00 a 19:00</v>
@@ -2828,7 +2828,7 @@
         <v>Domingo Cerrado</v>
       </c>
       <c r="Q24" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R24" t="str">
         <v>tepic</v>
@@ -2840,10 +2840,10 @@
         <v>https://www.google.com/maps/place/Mi+Hogar+Vivero/@21.5154489,-104.9196507,17z/data=!3m1!4b1!4m6!3m5!1s0x842737e99067082d:0x2e239f5d7fa495e!8m2!3d21.5154489!4d-104.9196507!16s%2Fg%2F11pv3p5b3r?authuser=0&amp;hl=es</v>
       </c>
       <c r="U24" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.8026445142928!2d-104.91965069999999!3d21.5154489!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842737e99067082d%3A0x2e239f5d7fa495e!2sMi%20Hogar%20Vivero!5e0!3m2!1ses!2smx!4v1681320260823!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.8026445142928!2d-104.91965069999999!3d21.5154489!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842737e99067082d%3A0x2e239f5d7fa495e!2sMi%20Hogar%20Vivero!5e0!3m2!1ses!2smx!4v1681340245823!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V24" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>G38J+54 Tepic, Nayarit</v>
       </c>
       <c r="W24" t="str">
         <v>0.0</v>
@@ -2926,7 +2926,7 @@
         <v>https://www.google.com/maps/place/Los+Viveros,+63037+Tepic,+Nay./@21.5266574,-104.8790715,18z/data=!3m1!4b1!4m6!3m5!1s0x842737a534de595b:0x8b387902469df4ce!8m2!3d21.5274988!4d-104.8788472!16s%2Fg%2F1tfvzgd2?authuser=0&amp;hl=es</v>
       </c>
       <c r="U25" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d1855.7581600716137!2d-104.87907154999999!3d21.5266574!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842737a534de595b%3A0x8b387902469df4ce!2sLos%20Viveros%2C%2063037%20Tepic%2C%20Nay.!5e0!3m2!1ses!2smx!4v1681320265140!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d1855.7581600716137!2d-104.87907154999999!3d21.5266574!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842737a534de595b%3A0x8b387902469df4ce!2sLos%20Viveros%2C%2063037%20Tepic%2C%20Nay.!5e0!3m2!1ses!2smx!4v1681340249959!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V25" t="str">
         <v>No cuenta con ciudad</v>
@@ -2988,10 +2988,10 @@
         <v>Lázaro Cárdenas 31, Adolfo López Mateos, 63021 Tepic, Nay.</v>
       </c>
       <c r="F26" t="str">
-        <v>G3CR+WJ Tepic, Nayarit</v>
+        <v>311 105 4961</v>
       </c>
       <c r="G26" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="I26" t="str">
         <v>Miércoles de 11:00 a 18:00,Jueves de 11:00 a 18:00,Viernes de 11:00 a 18:00,Sábado de 11:00 a 17:00,Domingo de 12:00 a 17:00,Lunes de 11:00 a 18:00,Martes de 11:00 a 18:00</v>
@@ -3018,7 +3018,7 @@
         <v>Domingo de 12:00 a 17:00</v>
       </c>
       <c r="Q26" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R26" t="str">
         <v>tepic</v>
@@ -3030,10 +3030,10 @@
         <v>https://www.google.com/maps/place/Mi+huerto+radio/@21.5222939,-104.908458,17z/data=!3m1!4b1!4m6!3m5!1s0x8427370c557ae413:0x36c273fffb8f2150!8m2!3d21.5222939!4d-104.908458!16s%2Fg%2F11p_7w1rlf?authuser=0&amp;hl=es</v>
       </c>
       <c r="U26" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.627803896471!2d-104.908458!3d21.522293899999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427370c557ae413%3A0x36c273fffb8f2150!2sMi%20huerto%20radio!5e0!3m2!1ses!2smx!4v1681320269492!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.627803896471!2d-104.908458!3d21.522293899999998!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427370c557ae413%3A0x36c273fffb8f2150!2sMi%20huerto%20radio!5e0!3m2!1ses!2smx!4v1681340254718!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V26" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>G3CR+WJ Tepic, Nayarit</v>
       </c>
       <c r="W26" t="str">
         <v>0.0</v>
@@ -3116,7 +3116,7 @@
         <v>https://www.google.com/maps/place/Saudades+vivero+literario/@21.4914401,-104.8854114,17z/data=!3m1!4b1!4m6!3m5!1s0x8427373c042f1a75:0x30a50c46e51b6038!8m2!3d21.4914401!4d-104.8854114!16s%2Fg%2F11nrw42m8b?authuser=0&amp;hl=es</v>
       </c>
       <c r="U27" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.4154782242686!2d-104.88541140000001!3d21.491440100000002!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427373c042f1a75%3A0x30a50c46e51b6038!2sSaudades%20vivero%20literario!5e0!3m2!1ses!2smx!4v1681320274431!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.4154782242686!2d-104.88541140000001!3d21.491440100000002!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427373c042f1a75%3A0x30a50c46e51b6038!2sSaudades%20vivero%20literario!5e0!3m2!1ses!2smx!4v1681340258361!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V27" t="str">
         <v>F4R7+HR Tepic, Nayarit</v>
@@ -3178,10 +3178,10 @@
         <v>aventida de la cultura 81 ciudad del valle Malaga, 63157 Tepic, Nay.</v>
       </c>
       <c r="F28" t="str">
-        <v>F4P9+J7 Tepic, Nayarit</v>
+        <v>311 214 3879</v>
       </c>
       <c r="G28" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="H28" t="str">
         <v>No se cuenta con horario oficial</v>
@@ -3190,7 +3190,7 @@
         <v>No se cuenta con horario oficial</v>
       </c>
       <c r="Q28" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R28" t="str">
         <v>tepic</v>
@@ -3202,10 +3202,10 @@
         <v>https://www.google.com/maps/place/Proximamente/@21.4865314,-104.8818174,17z/data=!3m1!4b1!4m6!3m5!1s0x8427376392d95471:0x6869282c8b63bce0!8m2!3d21.4865314!4d-104.8818174!16s%2Fg%2F11j7f9gqz4?authuser=0&amp;hl=es</v>
       </c>
       <c r="U28" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.540694392029!2d-104.88181739999999!3d21.4865314!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427376392d95471%3A0x6869282c8b63bce0!2sProximamente!5e0!3m2!1ses!2smx!4v1681320278626!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.540694392029!2d-104.88181739999999!3d21.4865314!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427376392d95471%3A0x6869282c8b63bce0!2sProximamente!5e0!3m2!1ses!2smx!4v1681340263311!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V28" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>F4P9+J7 Tepic, Nayarit</v>
       </c>
       <c r="W28" t="str">
         <v>0.0</v>
@@ -3264,10 +3264,10 @@
         <v>CUARZO AZUL 13, Fraccionamiento El Olimpo, 63173 Tepic, Nay.</v>
       </c>
       <c r="F29" t="str">
-        <v>F5V8+5M Tepic, Nayarit</v>
+        <v>311 249 5345</v>
       </c>
       <c r="G29" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="I29" t="str">
         <v>Miércoles de 10:00 a 05:00,Jueves de 10:00 a 05:00,Viernes de 10:00 a 05:00,Sábado de 10:00 a 14:00,Domingo Cerrado,Lunes de 10:00 a 05:00,Martes de 10:00 a 05:00</v>
@@ -3294,7 +3294,7 @@
         <v>Domingo Cerrado</v>
       </c>
       <c r="Q29" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R29" t="str">
         <v>tepic</v>
@@ -3306,10 +3306,10 @@
         <v>https://www.google.com/maps/place/vivero+SalvaTerra/@21.4929468,-104.8333375,17z/data=!3m1!4b1!4m6!3m5!1s0x84273945ca28fadf:0x8da9a8847756a881!8m2!3d21.4929468!4d-104.8333375!16s%2Fg%2F11nmj712gr?authuser=0&amp;hl=es</v>
       </c>
       <c r="U29" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.377038305595!2d-104.8333375!3d21.492946800000002!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273945ca28fadf%3A0x8da9a8847756a881!2svivero%20SalvaTerra!5e0!3m2!1ses!2smx!4v1681320282533!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.377038305595!2d-104.8333375!3d21.492946800000002!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273945ca28fadf%3A0x8da9a8847756a881!2svivero%20SalvaTerra!5e0!3m2!1ses!2smx!4v1681340268331!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V29" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>F5V8+5M Tepic, Nayarit</v>
       </c>
       <c r="W29" t="str">
         <v>1.0</v>
@@ -3410,7 +3410,7 @@
         <v>https://www.google.com/maps/place/Vivero+el+aeropuerto+Tepic/@21.4222744,-104.8303474,17z/data=!3m1!4b1!4m6!3m5!1s0x84273b819e9bf17d:0x593c17d07edba263!8m2!3d21.4222744!4d-104.8303474!16s%2Fg%2F11r6wr777s?authuser=0&amp;hl=es</v>
       </c>
       <c r="U30" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3714.177314604269!2d-104.8303474!3d21.4222744!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273b819e9bf17d%3A0x593c17d07edba263!2sVivero%20el%20aeropuerto%20Tepic!5e0!3m2!1ses!2smx!4v1681320286894!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3714.177314604269!2d-104.8303474!3d21.4222744!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273b819e9bf17d%3A0x593c17d07edba263!2sVivero%20el%20aeropuerto%20Tepic!5e0!3m2!1ses!2smx!4v1681340272398!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V30" t="str">
         <v>C5C9+WV Tepic, Nayarit</v>
@@ -3514,7 +3514,7 @@
         <v>https://www.google.com/maps/place/Sucacto+Tepic/@21.5354453,-104.9394221,17z/data=!3m1!4b1!4m6!3m5!1s0x84273766974786a9:0x6b7e78110b80bc6e!8m2!3d21.5354453!4d-104.9394221!16s%2Fg%2F11rpd9mn0b?authuser=0&amp;hl=es</v>
       </c>
       <c r="U31" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.2917313605585!2d-104.9394221!3d21.5354453!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273766974786a9%3A0x6b7e78110b80bc6e!2sSucacto%20Tepic!5e0!3m2!1ses!2smx!4v1681320291090!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.2917313605585!2d-104.9394221!3d21.5354453!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273766974786a9%3A0x6b7e78110b80bc6e!2sSucacto%20Tepic!5e0!3m2!1ses!2smx!4v1681340278807!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V31" t="str">
         <v>G3P6+56 Tepic, Nayarit</v>
@@ -3576,10 +3576,10 @@
         <v>63504 san Cayetano, 63504 Tepic, Nay.</v>
       </c>
       <c r="F32" t="str">
-        <v>C5XJ+RV Tepic, Nayarit</v>
+        <v>311 270 5526</v>
       </c>
       <c r="G32" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="I32" t="str">
         <v>Miércoles de 06:00 a 09:30,Jueves de 06:00 a 09:30,Viernes de 05:00 a 09:30,Sábado Abierto las 24 horas,Domingo Abierto las 24 horas,Lunes de 06:00 a 09:30,Martes de 06:00 a 09:30</v>
@@ -3606,7 +3606,7 @@
         <v>Domingo Abierto las 24 horas</v>
       </c>
       <c r="Q32" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R32" t="str">
         <v>tepic</v>
@@ -3618,10 +3618,10 @@
         <v>https://www.google.com/maps/place/viviero+contreras/@21.4495376,-104.8178373,17z/data=!3m1!4b1!4m6!3m5!1s0x84273b244d095ead:0xfc8365c6092a2d9a!8m2!3d21.4495376!4d-104.8178373!16s%2Fg%2F11tmwd4747?authuser=0&amp;hl=es</v>
       </c>
       <c r="U32" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3713.4834936967977!2d-104.8178373!3d21.449537599999996!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273b244d095ead%3A0xfc8365c6092a2d9a!2sviviero%20contreras!5e0!3m2!1ses!2smx!4v1681320295836!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3713.4834936967977!2d-104.8178373!3d21.449537599999996!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273b244d095ead%3A0xfc8365c6092a2d9a!2sviviero%20contreras!5e0!3m2!1ses!2smx!4v1681340284575!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V32" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>C5XJ+RV Tepic, Nayarit</v>
       </c>
       <c r="W32" t="str">
         <v>0.0</v>
@@ -3722,7 +3722,7 @@
         <v>https://www.google.com/maps/place/Vivero+V.+Carranza/@21.5199593,-104.9821969,17z/data=!3m1!4b1!4m6!3m5!1s0x8427358ee14b6c8b:0xb89ce65d42903111!8m2!3d21.5199593!4d-104.9821969!16s%2Fg%2F11pz7lhx2r?authuser=0&amp;hl=es</v>
       </c>
       <c r="U33" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.687442121995!2d-104.98219689999999!3d21.5199593!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427358ee14b6c8b%3A0xb89ce65d42903111!2sVivero%20V.%20Carranza!5e0!3m2!1ses!2smx!4v1681320299750!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.687442121995!2d-104.98219689999999!3d21.5199593!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427358ee14b6c8b%3A0xb89ce65d42903111!2sVivero%20V.%20Carranza!5e0!3m2!1ses!2smx!4v1681340289194!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V33" t="str">
         <v>G299+X4 Tepic, Nayarit</v>
@@ -3808,7 +3808,7 @@
         <v>https://www.google.com/maps/place/Huerta+%22AGUA+FR%C3%8DA%22+Vivero/@21.5566009,-104.9508409,17z/data=!3m1!4b1!4m6!3m5!1s0x84274b9b0647d475:0x5a0136474e73341a!8m2!3d21.5566009!4d-104.9508409!16s%2Fg%2F11nnvjpj20?authuser=0&amp;hl=es</v>
       </c>
       <c r="U34" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3710.750708236073!2d-104.95084089999999!3d21.556600899999996!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84274b9b0647d475%3A0x5a0136474e73341a!2sHuerta%20%22AGUA%20FR%C3%8DA%22%20Vivero!5e0!3m2!1ses!2smx!4v1681320303854!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3710.750708236073!2d-104.95084089999999!3d21.556600899999996!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84274b9b0647d475%3A0x5a0136474e73341a!2sHuerta%20%22AGUA%20FR%C3%8DA%22%20Vivero!5e0!3m2!1ses!2smx!4v1681340293935!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V34" t="str">
         <v>H24X+JM Tepic, Nayarit</v>
@@ -3894,7 +3894,7 @@
         <v>https://www.google.com/maps/place/Vivero+Conafor/@21.4632582,-104.8077903,17z/data=!3m1!4b1!4m6!3m5!1s0x84273bcad55e9f5d:0x57cab2a2f06bc0c5!8m2!3d21.4632582!4d-104.8077903!16s%2Fg%2F11c6vgq_1r?authuser=0&amp;hl=es</v>
       </c>
       <c r="U35" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3713.134000225909!2d-104.8077903!3d21.463258200000002!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273bcad55e9f5d%3A0x57cab2a2f06bc0c5!2sVivero%20Conafor!5e0!3m2!1ses!2smx!4v1681320308263!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3713.134000225909!2d-104.8077903!3d21.463258200000002!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273bcad55e9f5d%3A0x57cab2a2f06bc0c5!2sVivero%20Conafor!5e0!3m2!1ses!2smx!4v1681340298672!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V35" t="str">
         <v>F57R+8V Tepic, Nayarit</v>
@@ -3998,7 +3998,7 @@
         <v>https://www.google.com/maps/place/Viveros+Habitat/@21.5189117,-104.9126785,17z/data=!3m1!4b1!4m6!3m5!1s0x8427365dd0dc2ad1:0x1d22841935569827!8m2!3d21.5189117!4d-104.9126785!16s%2Fg%2F11bz_ym0k5?authuser=0&amp;hl=es</v>
       </c>
       <c r="U36" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.7142014506853!2d-104.9126785!3d21.5189117!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427365dd0dc2ad1%3A0x1d22841935569827!2sViveros%20Habitat!5e0!3m2!1ses!2smx!4v1681320312734!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.7142014506853!2d-104.9126785!3d21.5189117!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x8427365dd0dc2ad1%3A0x1d22841935569827!2sViveros%20Habitat!5e0!3m2!1ses!2smx!4v1681340303136!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V36" t="str">
         <v>G39P+HW Tepic, Nayarit</v>
@@ -4084,7 +4084,7 @@
         <v>https://www.google.com/maps/place/Viveros+Banquetes+Tepic/@21.3876969,-105.054392,11z/data=!3m1!4b1!4m6!3m5!1s0x842737afc548eb1b:0x1e70c90e1ed86049!8m2!3d21.387697!4d-105.054392!16s%2Fg%2F11pqxnnln4?authuser=0&amp;hl=es</v>
       </c>
       <c r="U37" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d237763.58823247807!2d-105.05439199999999!3d21.38769695!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842737afc548eb1b%3A0x1e70c90e1ed86049!2sViveros%20Banquetes%20Tepic!5e0!3m2!1ses!2smx!4v1681320317174!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d237763.58823247807!2d-105.05439199999999!3d21.38769695!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x842737afc548eb1b%3A0x1e70c90e1ed86049!2sViveros%20Banquetes%20Tepic!5e0!3m2!1ses!2smx!4v1681340307310!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V37" t="str">
         <v>311 190 7474</v>
@@ -4171,7 +4171,7 @@
         <v>https://www.google.com/maps/place/Vivero,+63511+San+Cayetano,+Nay./@21.4518169,-104.8147102,17z/data=!3m1!4b1!4m6!3m5!1s0x84273a389fa34965:0x28cde3b8ddf534ca!8m2!3d21.4510077!4d-104.8140899!16s%2Fg%2F11b8tfvznd?authuser=0&amp;hl=es</v>
       </c>
       <c r="U38" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3713.425450999701!2d-104.8147102!3d21.45181685!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273a389fa34965%3A0x28cde3b8ddf534ca!2sVivero%2C%2063511%20San%20Cayetano%2C%20Nay.!5e0!3m2!1ses!2smx!4v1681320321226!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3713.425450999701!2d-104.8147102!3d21.45181685!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273a389fa34965%3A0x28cde3b8ddf534ca!2sVivero%2C%2063511%20San%20Cayetano%2C%20Nay.!5e0!3m2!1ses!2smx!4v1681340311327!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V38" t="str">
         <v>No cuenta con ciudad</v>
@@ -4233,10 +4233,10 @@
         <v>Margaritas, Flor de Loto esquina, Jardines del Valle, 63035 Tepic, Nay.</v>
       </c>
       <c r="F39" t="str">
-        <v>G4HJ+W7 Tepic, Nayarit</v>
+        <v>311 300 5101</v>
       </c>
       <c r="G39" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="I39" t="str">
         <v>Miércoles de 08:00 a 20:00,Jueves de 08:00 a 20:00,Viernes de 08:00 a 20:00,Sábado Cerrado,Domingo Cerrado,Lunes de 08:00 a 20:00,Martes de 08:00 a 20:00</v>
@@ -4263,7 +4263,7 @@
         <v>Domingo Cerrado</v>
       </c>
       <c r="Q39" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R39" t="str">
         <v>tepic</v>
@@ -4275,10 +4275,10 @@
         <v>https://www.google.com/maps/place/PORFIRIO+planta/@21.5298233,-104.869267,17z/data=!3m1!4b1!4m6!3m5!1s0x84273782e16fedcf:0xa9ca5b0d1a3e57fd!8m2!3d21.5298233!4d-104.869267!16s%2Fg%2F11h70q_qrb?authuser=0&amp;hl=es</v>
       </c>
       <c r="U39" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.43542058705!2d-104.869267!3d21.529823299999997!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273782e16fedcf%3A0xa9ca5b0d1a3e57fd!2sPORFIRIO%20planta!5e0!3m2!1ses!2smx!4v1681320325040!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3711.43542058705!2d-104.869267!3d21.529823299999997!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273782e16fedcf%3A0xa9ca5b0d1a3e57fd!2sPORFIRIO%20planta!5e0!3m2!1ses!2smx!4v1681340315311!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V39" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>G4HJ+W7 Tepic, Nayarit</v>
       </c>
       <c r="W39" t="str">
         <v>0.0</v>
@@ -4337,10 +4337,10 @@
         <v>Av. Universidad 134, Cd del Valle, 63157 Tepic, Nay.</v>
       </c>
       <c r="F40" t="str">
-        <v>F4R7+67 Tepic, Nayarit</v>
+        <v>311 213 9710</v>
       </c>
       <c r="G40" t="str">
-        <v/>
+        <v>Web no disponible</v>
       </c>
       <c r="H40" t="str">
         <v>No se cuenta con horario oficial</v>
@@ -4349,7 +4349,7 @@
         <v>No se cuenta con horario oficial</v>
       </c>
       <c r="Q40" t="str">
-        <v xml:space="preserve"> tu teléfono</v>
+        <v>Tepic, Nayarit</v>
       </c>
       <c r="R40" t="str">
         <v>tepic</v>
@@ -4361,10 +4361,10 @@
         <v>https://www.google.com/maps/place/Pineda+Viveros+y+Asociados/@21.4906185,-104.886816,17z/data=!3m1!4b1!4m6!3m5!1s0x84273721f3de9809:0xeab8568f1cdc676d!8m2!3d21.4906185!4d-104.886816!16s%2Fg%2F1v9gvsm9?authuser=0&amp;hl=es</v>
       </c>
       <c r="U40" t="str">
-        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.4364383407383!2d-104.886816!3d21.490618500000004!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273721f3de9809%3A0xeab8568f1cdc676d!2sPineda%20Viveros%20y%20Asociados!5e0!3m2!1ses!2smx!4v1681320330299!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3712.4364383407383!2d-104.886816!3d21.490618500000004!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x84273721f3de9809%3A0xeab8568f1cdc676d!2sPineda%20Viveros%20y%20Asociados!5e0!3m2!1ses!2smx!4v1681340320316!5m2!1ses!2smx" width="390" height="420" style="border:0;" allowfullscreen="" loading="lazy" referrerpolicy="no-referrer-when-downgrade"&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="V40" t="str">
-        <v>Enviar a tu teléfono</v>
+        <v>F4R7+67 Tepic, Nayarit</v>
       </c>
       <c r="W40" t="str">
         <v>5.0</v>

</xml_diff>